<commit_message>
update mock XLSX file
</commit_message>
<xml_diff>
--- a/modules/veteran/spec/fixtures/xlsx_files/rep-mock-data.xlsx
+++ b/modules/veteran/spec/fixtures/xlsx_files/rep-mock-data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="145">
   <si>
     <t>Number</t>
   </si>
@@ -117,130 +117,97 @@
     <t>TX</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>email_with_trailing_whitespace@example.com</t>
-    </r>
+    <t xml:space="preserve">email_with_trailing_whitespace@example.com </t>
+  </si>
+  <si>
+    <t>07Z</t>
+  </si>
+  <si>
+    <t>Boardroom</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>1 Chemical Corporate</t>
+  </si>
+  <si>
+    <t>Suite 100</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>1I4</t>
+  </si>
+  <si>
+    <t>Mal</t>
+  </si>
+  <si>
+    <t>Stewart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Law Offices of Beavis &amp; Stein, P.C. </t>
+  </si>
+  <si>
+    <t>400 W. Nard Avenue</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
+  </si>
+  <si>
+    <t>01H</t>
+  </si>
+  <si>
+    <t>Bestward</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Road &amp; Pond, P.A.</t>
+  </si>
+  <si>
+    <t>P.O. Box 100</t>
+  </si>
+  <si>
+    <t>Deland</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t>name@name@example.com</t>
     </r>
   </si>
   <si>
-    <t>07Z</t>
-  </si>
-  <si>
-    <t>Boardroom</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Mr.</t>
-  </si>
-  <si>
-    <t>1 Chemical Corporate</t>
-  </si>
-  <si>
-    <t>Suite 100</t>
-  </si>
-  <si>
-    <t>Birmingham</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>1I4</t>
-  </si>
-  <si>
-    <t>Mal</t>
-  </si>
-  <si>
-    <t>Stewart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Law Offices of Beavis &amp; Stein, P.C. </t>
-  </si>
-  <si>
-    <t>400 W. Nard Avenue</t>
-  </si>
-  <si>
-    <t>Albany</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>www.google.com</t>
-    </r>
-  </si>
-  <si>
-    <t>01H</t>
-  </si>
-  <si>
-    <t>Bestward</t>
-  </si>
-  <si>
-    <t>Steven</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Road &amp; Pond, P.A.</t>
-  </si>
-  <si>
-    <t>P.O. Box 100</t>
-  </si>
-  <si>
-    <t>Deland</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>name@</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>name@example.com</t>
-    </r>
-  </si>
-  <si>
     <t>WorkEmailAddress</t>
   </si>
   <si>
@@ -301,15 +268,7 @@
     <t>44077-0490</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>first_last@example.com</t>
-    </r>
+    <t>first_last@example.com</t>
   </si>
   <si>
     <t>Veterans of Foreign Wars</t>
@@ -364,17 +323,6 @@
   </si>
   <si>
     <t>ASDF</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>email_with_trailing_whitespace@example.com</t>
-    </r>
   </si>
   <si>
     <t>G</t>
@@ -516,7 +464,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -530,12 +478,6 @@
     <font>
       <sz val="15"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -623,7 +565,6 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1975,11 +1916,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="P3" r:id="rId1" location="" tooltip="" display="email_with_trailing_whitespace@example.com"/>
-    <hyperlink ref="P5" r:id="rId2" location="" tooltip="" display="www.google.com"/>
-    <hyperlink ref="P6" r:id="rId3" location="" tooltip="" display="name@example.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -2009,7 +1945,7 @@
     <col min="11" max="11" width="11.5" style="5" customWidth="1"/>
     <col min="12" max="12" width="18" style="5" customWidth="1"/>
     <col min="13" max="13" width="21.1719" style="5" customWidth="1"/>
-    <col min="14" max="14" width="36.5" style="5" customWidth="1"/>
+    <col min="14" max="14" width="51.1094" style="5" customWidth="1"/>
     <col min="15" max="15" width="49.6719" style="5" customWidth="1"/>
     <col min="16" max="16" width="19.8516" style="5" customWidth="1"/>
     <col min="17" max="17" width="9.5" style="5" customWidth="1"/>
@@ -2901,7 +2837,7 @@
         <v>25</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>72</v>
@@ -2952,7 +2888,7 @@
         <v>25</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>84</v>
@@ -2975,25 +2911,25 @@
         <v>47</v>
       </c>
       <c r="D19" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="E19" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="E19" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="F19" t="s" s="2">
+      <c r="G19" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="G19" t="s" s="2">
+      <c r="H19" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="H19" t="s" s="2">
+      <c r="I19" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="I19" t="s" s="2">
+      <c r="J19" t="s" s="2">
         <v>106</v>
-      </c>
-      <c r="J19" t="s" s="2">
-        <v>107</v>
       </c>
       <c r="K19" s="3">
         <v>10014</v>
@@ -3028,25 +2964,25 @@
         <v>55</v>
       </c>
       <c r="D20" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="E20" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="E20" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="F20" t="s" s="2">
+      <c r="G20" t="s" s="2">
         <v>109</v>
       </c>
-      <c r="G20" t="s" s="2">
+      <c r="H20" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="I20" t="s" s="2">
         <v>110</v>
       </c>
-      <c r="H20" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I20" t="s" s="2">
+      <c r="J20" t="s" s="2">
         <v>111</v>
-      </c>
-      <c r="J20" t="s" s="2">
-        <v>112</v>
       </c>
       <c r="K20" s="3">
         <v>25701</v>
@@ -3061,7 +2997,7 @@
         <v>44</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P20" s="3">
         <v>1</v>
@@ -3071,16 +3007,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" location="" tooltip="" display="first_last@example.com"/>
-    <hyperlink ref="N4" r:id="rId2" location="" tooltip="" display="first_last@example.com"/>
-    <hyperlink ref="N5" r:id="rId3" location="" tooltip="" display="first_last@example.com"/>
-    <hyperlink ref="N6" r:id="rId4" location="" tooltip="" display="first_last@example.com"/>
-    <hyperlink ref="N7" r:id="rId5" location="" tooltip="" display="first_last@example.com"/>
-    <hyperlink ref="N8" r:id="rId6" location="" tooltip="" display="first_last@example.com"/>
-    <hyperlink ref="N17" r:id="rId7" location="" tooltip="" display="email_with_trailing_whitespace@example.com"/>
-    <hyperlink ref="N18" r:id="rId8" location="" tooltip="" display="email_with_trailing_whitespace@example.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -3119,31 +3045,31 @@
         <v>1</v>
       </c>
       <c r="C1" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s" s="2">
         <v>114</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="E1" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="F1" t="s" s="2">
         <v>116</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="G1" t="s" s="2">
         <v>117</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="H1" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="I1" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="J1" t="s" s="2">
         <v>120</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="K1" t="s" s="2">
         <v>121</v>
-      </c>
-      <c r="K1" t="s" s="2">
-        <v>122</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
@@ -3154,25 +3080,25 @@
         <v>80</v>
       </c>
       <c r="C2" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="E2" t="s" s="2">
         <v>124</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="F2" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="F2" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s" s="2">
+      <c r="I2" t="s" s="2">
         <v>126</v>
-      </c>
-      <c r="I2" t="s" s="2">
-        <v>127</v>
       </c>
       <c r="J2" s="3">
         <v>22314</v>
@@ -3189,28 +3115,28 @@
         <v>85</v>
       </c>
       <c r="C3" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s" s="2">
         <v>128</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="E3" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="F3" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="I3" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="J3" t="s" s="2">
         <v>130</v>
-      </c>
-      <c r="F3" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="I3" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="J3" t="s" s="2">
-        <v>131</v>
       </c>
       <c r="K3" s="3">
         <v>1</v>
@@ -3224,25 +3150,25 @@
         <v>91</v>
       </c>
       <c r="C4" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="D4" t="s" s="2">
         <v>132</v>
       </c>
-      <c r="D4" t="s" s="2">
+      <c r="E4" t="s" s="2">
         <v>133</v>
       </c>
-      <c r="E4" t="s" s="2">
+      <c r="F4" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s" s="2">
         <v>134</v>
       </c>
-      <c r="F4" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s" s="2">
+      <c r="I4" t="s" s="2">
         <v>135</v>
-      </c>
-      <c r="I4" t="s" s="2">
-        <v>136</v>
       </c>
       <c r="J4" s="3">
         <v>98498</v>
@@ -3259,22 +3185,22 @@
         <v>65</v>
       </c>
       <c r="C5" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="E5" t="s" s="2">
         <v>138</v>
       </c>
-      <c r="E5" t="s" s="2">
+      <c r="F5" t="s" s="2">
         <v>139</v>
       </c>
-      <c r="F5" t="s" s="2">
+      <c r="G5" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s" s="2">
         <v>140</v>
-      </c>
-      <c r="G5" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>141</v>
       </c>
       <c r="I5" t="s" s="2">
         <v>33</v>
@@ -3294,22 +3220,22 @@
         <v>74</v>
       </c>
       <c r="C6" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="D6" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="D6" t="s" s="2">
+      <c r="E6" t="s" s="2">
         <v>143</v>
       </c>
-      <c r="E6" t="s" s="2">
+      <c r="F6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s" s="2">
         <v>144</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>145</v>
       </c>
       <c r="I6" t="s" s="2">
         <v>24</v>

</xml_diff>